<commit_message>
some zoop analyses and spring/fall comparisons
</commit_message>
<xml_diff>
--- a/PHaseIV analyses.xlsx
+++ b/PHaseIV analyses.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\phaseIV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\FRPreport2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE305C2C-69F2-4837-8A78-AEEABB16B778}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7920" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise" sheetId="1" r:id="rId1"/>
     <sheet name="everything" sheetId="2" r:id="rId2"/>
+    <sheet name="spring v fall" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="164">
   <si>
     <t>---</t>
   </si>
@@ -436,12 +444,93 @@
   </si>
   <si>
     <t>Intercept - Site: Channel, Gear: Mysid, Region: Grizzly</t>
+  </si>
+  <si>
+    <t>Call:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lm(formula = log(tCPUE) ~ site + targets2 + season, data = bugsblitzSF.1[which(bugsblitzSF.1$SampleID != </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "MAC6-22MAR2018"), ])</t>
+  </si>
+  <si>
+    <t>Residuals:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.3307 -1.3386 -0.1527  1.1829  4.0837 </t>
+  </si>
+  <si>
+    <t>Coefficients:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Estimate Std. Error t value Pr(&gt;|t|)  </t>
+  </si>
+  <si>
+    <t>(Intercept)         1.4008     0.5835   2.401   0.0192 *</t>
+  </si>
+  <si>
+    <t>siteBrowns         -1.5584     0.6896  -2.260   0.0272 *</t>
+  </si>
+  <si>
+    <t>siteWinter         -1.2670     0.7046  -1.798   0.0768 .</t>
+  </si>
+  <si>
+    <t>siteProspect        1.6347     0.6740   2.425   0.0181 *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">targets2sweep net   0.4973     0.5075   0.980   0.3307  </t>
+  </si>
+  <si>
+    <t>seasonfall          1.0949     0.5002   2.189   0.0322 *</t>
+  </si>
+  <si>
+    <t>Signif. codes:  0 ‘***’ 0.001 ‘**’ 0.01 ‘*’ 0.05 ‘.’ 0.1 ‘ ’ 1</t>
+  </si>
+  <si>
+    <t>Residual standard error: 2.018 on 65 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple R-squared:  0.3436,    Adjusted R-squared:  0.2931 </t>
+  </si>
+  <si>
+    <t>F-statistic: 6.805 on 5 and 65 DF,  p-value: 3.692e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adonis(formula = sf.12p ~ site + targets2 + season, data = sf2) </t>
+  </si>
+  <si>
+    <t>Permutation: free</t>
+  </si>
+  <si>
+    <t>Number of permutations: 999</t>
+  </si>
+  <si>
+    <t>Terms added sequentially (first to last)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Df SumsOfSqs MeanSqs F.Model      R2 Pr(&gt;F)    </t>
+  </si>
+  <si>
+    <t>site       3    4.6812 1.56039 10.0981 0.25666  0.001 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">targets2   1    0.5781 0.57806  3.7409 0.03169  0.011 *  </t>
+  </si>
+  <si>
+    <t>season     1    2.7813 2.78127 17.9990 0.15249  0.001 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residuals 66   10.1986 0.15452         0.55916           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total     71   18.2391                 1.00000           </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -885,24 +974,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>1</v>
@@ -920,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -943,7 +1032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -966,7 +1055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -986,7 +1075,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1000,96 +1089,96 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>1</v>
@@ -1110,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1136,7 +1225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -1188,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1294,7 @@
         <v>0.62258000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1226,19 +1315,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="K148" sqref="K148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" t="s">
         <v>1</v>
@@ -1259,7 +1348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1285,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1311,7 +1400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1337,7 +1426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1381,7 +1470,7 @@
         <v>0.67588999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1395,74 +1484,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>68</v>
       </c>
@@ -1470,7 +1559,7 @@
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
         <v>54</v>
@@ -1480,7 +1569,7 @@
       </c>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
@@ -1494,10 +1583,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>67</v>
       </c>
@@ -1505,7 +1594,7 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="9" t="s">
         <v>54</v>
@@ -1515,7 +1604,7 @@
       </c>
       <c r="D33" s="9"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>105</v>
       </c>
@@ -1529,7 +1618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
@@ -1543,7 +1632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
@@ -1557,7 +1646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>106</v>
       </c>
@@ -1571,7 +1660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -1585,7 +1674,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
@@ -1599,7 +1688,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>64</v>
       </c>
@@ -1613,7 +1702,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>65</v>
       </c>
@@ -1627,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>107</v>
       </c>
@@ -1641,7 +1730,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1655,7 +1744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>108</v>
       </c>
@@ -1669,7 +1758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -1683,7 +1772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>109</v>
       </c>
@@ -1697,7 +1786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -1711,7 +1800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>110</v>
       </c>
@@ -1725,7 +1814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
         <v>111</v>
       </c>
@@ -1739,10 +1828,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>69</v>
       </c>
@@ -1750,7 +1839,7 @@
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="9" t="s">
         <v>54</v>
@@ -1760,7 +1849,7 @@
       </c>
       <c r="D52" s="9"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>56</v>
       </c>
@@ -1774,7 +1863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -1788,7 +1877,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -1802,7 +1891,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>59</v>
       </c>
@@ -1816,7 +1905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -1830,7 +1919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>60</v>
       </c>
@@ -1844,10 +1933,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>70</v>
       </c>
@@ -1855,7 +1944,7 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="9" t="s">
         <v>54</v>
@@ -1865,7 +1954,7 @@
       </c>
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -1879,7 +1968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
@@ -1893,12 +1982,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>68</v>
       </c>
@@ -1906,7 +1995,7 @@
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" t="s">
         <v>54</v>
@@ -1915,7 +2004,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>66</v>
       </c>
@@ -1929,10 +2018,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>67</v>
       </c>
@@ -1940,7 +2029,7 @@
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="9" t="s">
         <v>54</v>
@@ -1950,7 +2039,7 @@
       </c>
       <c r="D73" s="9"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -1964,7 +2053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -1978,7 +2067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
@@ -1992,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
@@ -2006,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>76</v>
       </c>
@@ -2020,10 +2109,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>69</v>
       </c>
@@ -2031,7 +2120,7 @@
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" t="s">
         <v>54</v>
@@ -2040,7 +2129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>77</v>
       </c>
@@ -2054,7 +2143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>78</v>
       </c>
@@ -2068,10 +2157,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>70</v>
       </c>
@@ -2079,7 +2168,7 @@
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" t="s">
         <v>54</v>
@@ -2088,7 +2177,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
         <v>79</v>
       </c>
@@ -2102,84 +2191,84 @@
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" t="s">
         <v>92</v>
@@ -2197,7 +2286,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>97</v>
       </c>
@@ -2220,7 +2309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>98</v>
       </c>
@@ -2243,7 +2332,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>99</v>
       </c>
@@ -2263,7 +2352,7 @@
         <v>0.14779999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>100</v>
       </c>
@@ -2283,7 +2372,7 @@
         <v>0.58250000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>101</v>
       </c>
@@ -2306,7 +2395,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>102</v>
       </c>
@@ -2329,84 +2418,84 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" t="s">
         <v>92</v>
@@ -2424,7 +2513,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>97</v>
       </c>
@@ -2447,7 +2536,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>98</v>
       </c>
@@ -2470,7 +2559,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>99</v>
       </c>
@@ -2490,7 +2579,7 @@
         <v>0.21551999999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>100</v>
       </c>
@@ -2510,7 +2599,7 @@
         <v>0.51256000000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>121</v>
       </c>
@@ -2530,7 +2619,7 @@
         <v>0.70955000000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>122</v>
       </c>
@@ -2550,7 +2639,7 @@
         <v>0.42113</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>123</v>
       </c>
@@ -2570,7 +2659,7 @@
         <v>0.53713</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>124</v>
       </c>
@@ -2590,7 +2679,7 @@
         <v>0.83803000000000005</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>125</v>
       </c>
@@ -2610,12 +2699,12 @@
         <v>0.82184000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="17"/>
       <c r="B148" s="18" t="s">
         <v>92</v>
@@ -2633,7 +2722,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>136</v>
       </c>
@@ -2656,7 +2745,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>127</v>
       </c>
@@ -2679,7 +2768,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>128</v>
       </c>
@@ -2699,7 +2788,7 @@
         <v>0.25020999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>129</v>
       </c>
@@ -2719,7 +2808,7 @@
         <v>0.63168999999999997</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>130</v>
       </c>
@@ -2739,7 +2828,7 @@
         <v>0.36756</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>131</v>
       </c>
@@ -2759,7 +2848,7 @@
         <v>0.46977000000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>132</v>
       </c>
@@ -2779,7 +2868,7 @@
         <v>0.98092000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>133</v>
       </c>
@@ -2799,7 +2888,7 @@
         <v>0.68081000000000003</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>134</v>
       </c>
@@ -2822,7 +2911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="20" t="s">
         <v>135</v>
       </c>
@@ -2843,6 +2932,185 @@
       </c>
       <c r="G158" t="s">
         <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1674AE-ACC1-453C-AA37-C3459A9647D0}">
+  <dimension ref="A2:A38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put all the pairwise comparisons on the powerpoit for the May 8th meeting
</commit_message>
<xml_diff>
--- a/PHaseIV analyses.xlsx
+++ b/PHaseIV analyses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\FRPreport2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE305C2C-69F2-4837-8A78-AEEABB16B778}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21C90B6-0D60-4AD7-9159-47D5943E3FF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="239">
   <si>
     <t>---</t>
   </si>
@@ -464,27 +464,6 @@
     <t>Coefficients:</t>
   </si>
   <si>
-    <t xml:space="preserve">                  Estimate Std. Error t value Pr(&gt;|t|)  </t>
-  </si>
-  <si>
-    <t>(Intercept)         1.4008     0.5835   2.401   0.0192 *</t>
-  </si>
-  <si>
-    <t>siteBrowns         -1.5584     0.6896  -2.260   0.0272 *</t>
-  </si>
-  <si>
-    <t>siteWinter         -1.2670     0.7046  -1.798   0.0768 .</t>
-  </si>
-  <si>
-    <t>siteProspect        1.6347     0.6740   2.425   0.0181 *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">targets2sweep net   0.4973     0.5075   0.980   0.3307  </t>
-  </si>
-  <si>
-    <t>seasonfall          1.0949     0.5002   2.189   0.0322 *</t>
-  </si>
-  <si>
     <t>Signif. codes:  0 ‘***’ 0.001 ‘**’ 0.01 ‘*’ 0.05 ‘.’ 0.1 ‘ ’ 1</t>
   </si>
   <si>
@@ -509,22 +488,268 @@
     <t>Terms added sequentially (first to last)</t>
   </si>
   <si>
-    <t xml:space="preserve">          Df SumsOfSqs MeanSqs F.Model      R2 Pr(&gt;F)    </t>
-  </si>
-  <si>
-    <t>site       3    4.6812 1.56039 10.0981 0.25666  0.001 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">targets2   1    0.5781 0.57806  3.7409 0.03169  0.011 *  </t>
-  </si>
-  <si>
-    <t>season     1    2.7813 2.78127 17.9990 0.15249  0.001 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residuals 66   10.1986 0.15452         0.55916           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total     71   18.2391                 1.00000           </t>
+    <t>Zooplankton CPUE</t>
+  </si>
+  <si>
+    <t>Linear mixed model fit by REML. t-tests use Satterthwaite's method ['lmerModLmerTest']</t>
+  </si>
+  <si>
+    <t>Formula: logCPUE ~ Region2 + sitetype2 + year + (1 | site)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Data: zootot</t>
+  </si>
+  <si>
+    <t>REML criterion at convergence: 474.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Min       1Q   Median       3Q      Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.16241 -0.60633  0.03806  0.58364  3.12087 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> site     (Intercept) 0.993    0.9965  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Residual             1.684    1.2978  </t>
+  </si>
+  <si>
+    <t>Number of obs: 138, groups:  site, 15</t>
+  </si>
+  <si>
+    <t>Correlation of Fixed Effects:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            (Intr) Rgn2Cn Rg2N-D R2S-SJ Rgn2SB sttyp2d sttyp2m sttyp2t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regn2Cnflnc -0.590                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rgn2Nrs-Dnv -0.604  0.454                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rgn2Sn-SnJq -0.591  0.506  0.451                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regin2SsnBy -0.624  0.468  0.586  0.464                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitetyp2dkd -0.142 -0.001 -0.290  0.002 -0.305                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitetyp2mtd -0.505  0.033  0.266  0.033  0.264  0.135                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitetyp2tdl -0.433 -0.003  0.034  0.008  0.012  0.327   0.413         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">year2018    -0.184  0.037 -0.060  0.043  0.016 -0.021  -0.009  -0.063 </t>
+  </si>
+  <si>
+    <t>Region2Nurse-Denverton</t>
+  </si>
+  <si>
+    <t>Region2San-San Joaquin</t>
+  </si>
+  <si>
+    <t>Region2Suisun Bay</t>
+  </si>
+  <si>
+    <t>sitetype2diked</t>
+  </si>
+  <si>
+    <t>sitetype2muted</t>
+  </si>
+  <si>
+    <t>sitetype2tidal</t>
+  </si>
+  <si>
+    <t>year2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adonis(formula = zMatp ~ Region2 + sitetype2 + year, data = zootot) </t>
+  </si>
+  <si>
+    <t>sitetype2</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>CLAMS</t>
+  </si>
+  <si>
+    <t>MACROINVERTS - log CPUE, best model by AICC with site as error term</t>
+  </si>
+  <si>
+    <t>targets2sweep net</t>
+  </si>
+  <si>
+    <t>&lt; 2e-16</t>
+  </si>
+  <si>
+    <t>siteBrowns</t>
+  </si>
+  <si>
+    <t>siteWinter</t>
+  </si>
+  <si>
+    <t>siteProspect</t>
+  </si>
+  <si>
+    <t>targets2sweep</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>seasonfall</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>Sacramento San Joaquin</t>
+  </si>
+  <si>
+    <t>Total Catch anova</t>
+  </si>
+  <si>
+    <t>&lt;2e-16</t>
+  </si>
+  <si>
+    <t>Year2</t>
+  </si>
+  <si>
+    <t>PERMANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adonis(formula = RegMat.12p ~ site + Year + targets2, data = Reg2) </t>
+  </si>
+  <si>
+    <t>Cache Slougjh</t>
+  </si>
+  <si>
+    <t>Df Sum Sq Mean Sq F</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>3  50.09   16.70</t>
+  </si>
+  <si>
+    <t>2 229.95  114.97</t>
+  </si>
+  <si>
+    <t>1  13.58   13.58</t>
+  </si>
+  <si>
+    <t>85 156.70    1.84</t>
+  </si>
+  <si>
+    <t>Df SumsOfSqs MeanSqs F.Model</t>
+  </si>
+  <si>
+    <t>R2 Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t>site       3    3.7805 1.26016  9.0941</t>
+  </si>
+  <si>
+    <t>0.20452  0.001</t>
+  </si>
+  <si>
+    <t>Year       1    0.4823 0.48233  3.4808</t>
+  </si>
+  <si>
+    <t>0.02609  0.019</t>
+  </si>
+  <si>
+    <t>targets2   2    2.4431 1.22156  8.8155</t>
+  </si>
+  <si>
+    <t>0.13217  0.001</t>
+  </si>
+  <si>
+    <t>Residuals 85   11.7784 0.13857</t>
+  </si>
+  <si>
+    <t>Total     91   18.4843</t>
+  </si>
+  <si>
+    <t>Confluence</t>
+  </si>
+  <si>
+    <t>Df S</t>
+  </si>
+  <si>
+    <t>umsOfSqs M</t>
+  </si>
+  <si>
+    <t>eanSqs F</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>f value</t>
+  </si>
+  <si>
+    <t>Suisun Bay</t>
+  </si>
+  <si>
+    <t>cache zooplankton permanoca</t>
+  </si>
+  <si>
+    <t>zooplankton anova</t>
+  </si>
+  <si>
+    <t>Clams ANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tukey multiple comparisons of means</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    95% family-wise confidence level</t>
+  </si>
+  <si>
+    <t>Fit: aov(formula = logCPUE ~ site, data = bensum)</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>lwr</t>
+  </si>
+  <si>
+    <t>upr</t>
+  </si>
+  <si>
+    <t>p adj</t>
+  </si>
+  <si>
+    <t>Prospect-Liberty</t>
+  </si>
+  <si>
+    <t>Miner-Liberty</t>
+  </si>
+  <si>
+    <t>Flyway-Liberty</t>
+  </si>
+  <si>
+    <t>Miner-Prospect</t>
+  </si>
+  <si>
+    <t>Flyway-Prospect</t>
+  </si>
+  <si>
+    <t>Flyway-Miner</t>
+  </si>
+  <si>
+    <t>CLAMS anova</t>
   </si>
 </sst>
 </file>
@@ -616,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -661,6 +886,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,15 +1203,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:Z125"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1308,18 +1538,1321 @@
         <v>1</v>
       </c>
     </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>193</v>
+      </c>
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>3</v>
+      </c>
+      <c r="N40" t="s">
+        <v>4</v>
+      </c>
+      <c r="O40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>15.26</v>
+      </c>
+      <c r="D41">
+        <v>7.63</v>
+      </c>
+      <c r="E41">
+        <v>3.74</v>
+      </c>
+      <c r="F41">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>24.89</v>
+      </c>
+      <c r="M41">
+        <v>12.443</v>
+      </c>
+      <c r="N41">
+        <v>2.423</v>
+      </c>
+      <c r="O41">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>291.85000000000002</v>
+      </c>
+      <c r="D42">
+        <v>145.91999999999999</v>
+      </c>
+      <c r="E42">
+        <v>71.540000000000006</v>
+      </c>
+      <c r="F42" t="s">
+        <v>194</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>4.47</v>
+      </c>
+      <c r="M42">
+        <v>4.4649999999999999</v>
+      </c>
+      <c r="N42">
+        <v>0.87</v>
+      </c>
+      <c r="O42">
+        <v>0.36599999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>5.46</v>
+      </c>
+      <c r="D43">
+        <v>5.46</v>
+      </c>
+      <c r="E43">
+        <v>2.6749999999999998</v>
+      </c>
+      <c r="F43">
+        <v>0.1053</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43">
+        <v>15</v>
+      </c>
+      <c r="L43">
+        <v>77.02</v>
+      </c>
+      <c r="M43">
+        <v>5.1340000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>93</v>
+      </c>
+      <c r="C44">
+        <v>189.7</v>
+      </c>
+      <c r="D44">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>1.4682999999999999</v>
+      </c>
+      <c r="D55">
+        <v>0.73416999999999999</v>
+      </c>
+      <c r="E55">
+        <v>5.7648000000000001</v>
+      </c>
+      <c r="F55">
+        <v>8.1269999999999995E-2</v>
+      </c>
+      <c r="G55">
+        <v>1E-3</v>
+      </c>
+      <c r="H55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0.70779999999999998</v>
+      </c>
+      <c r="D56">
+        <v>0.70782</v>
+      </c>
+      <c r="E56">
+        <v>5.5579000000000001</v>
+      </c>
+      <c r="F56">
+        <v>3.9170000000000003E-2</v>
+      </c>
+      <c r="G56">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>4.0480999999999998</v>
+      </c>
+      <c r="D57">
+        <v>2.02407</v>
+      </c>
+      <c r="E57">
+        <v>15.8933</v>
+      </c>
+      <c r="F57">
+        <v>0.22405</v>
+      </c>
+      <c r="G57">
+        <v>1E-3</v>
+      </c>
+      <c r="H57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>93</v>
+      </c>
+      <c r="C58">
+        <v>11.8439</v>
+      </c>
+      <c r="D58">
+        <v>0.12734999999999999</v>
+      </c>
+      <c r="F58">
+        <v>0.65551000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59">
+        <v>98</v>
+      </c>
+      <c r="C59">
+        <v>18.068200000000001</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67">
+        <v>9.0570000000000004</v>
+      </c>
+      <c r="D67" s="4">
+        <v>2.87E-5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68">
+        <v>62.366999999999997</v>
+      </c>
+      <c r="D68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="T68" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69">
+        <v>7.3639999999999999</v>
+      </c>
+      <c r="D69">
+        <v>8.0599999999999995E-3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>62</v>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="T69" s="2"/>
+      <c r="U69" t="s">
+        <v>1</v>
+      </c>
+      <c r="V69" t="s">
+        <v>2</v>
+      </c>
+      <c r="W69" t="s">
+        <v>3</v>
+      </c>
+      <c r="X69" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>204</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" t="s">
+        <v>1</v>
+      </c>
+      <c r="M70" t="s">
+        <v>28</v>
+      </c>
+      <c r="N70" t="s">
+        <v>29</v>
+      </c>
+      <c r="O70" t="s">
+        <v>30</v>
+      </c>
+      <c r="P70" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>5</v>
+      </c>
+      <c r="T70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U70">
+        <v>3</v>
+      </c>
+      <c r="V70">
+        <v>33.86</v>
+      </c>
+      <c r="W70">
+        <v>11.287000000000001</v>
+      </c>
+      <c r="X70">
+        <v>9.875</v>
+      </c>
+      <c r="Y70">
+        <v>6.5599999999999999E-3</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="K71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>1.3683000000000001</v>
+      </c>
+      <c r="N71">
+        <v>0.68415999999999999</v>
+      </c>
+      <c r="O71">
+        <v>4.6266999999999996</v>
+      </c>
+      <c r="P71">
+        <v>0.24396000000000001</v>
+      </c>
+      <c r="Q71">
+        <v>2E-3</v>
+      </c>
+      <c r="R71" t="s">
+        <v>62</v>
+      </c>
+      <c r="T71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U71">
+        <v>7</v>
+      </c>
+      <c r="V71">
+        <v>8</v>
+      </c>
+      <c r="W71">
+        <v>1.143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="K72" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>0.39579999999999999</v>
+      </c>
+      <c r="N72">
+        <v>0.39577000000000001</v>
+      </c>
+      <c r="O72">
+        <v>2.6764000000000001</v>
+      </c>
+      <c r="P72">
+        <v>7.0559999999999998E-2</v>
+      </c>
+      <c r="Q72">
+        <v>2.7E-2</v>
+      </c>
+      <c r="R72" t="s">
+        <v>32</v>
+      </c>
+      <c r="T72" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" t="s">
+        <v>206</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73">
+        <v>26</v>
+      </c>
+      <c r="M73">
+        <v>3.8447</v>
+      </c>
+      <c r="N73">
+        <v>0.14787</v>
+      </c>
+      <c r="P73">
+        <v>0.68547999999999998</v>
+      </c>
+      <c r="T73" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B74" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L74">
+        <v>29</v>
+      </c>
+      <c r="M74">
+        <v>5.6087999999999996</v>
+      </c>
+      <c r="P74">
+        <v>1</v>
+      </c>
+      <c r="T74" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" t="s">
+        <v>32</v>
+      </c>
+      <c r="T75" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B76" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="T76" s="1"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B77">
+        <v>0.63721000000000005</v>
+      </c>
+      <c r="K77" t="s">
+        <v>223</v>
+      </c>
+      <c r="T77" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="K78" s="2"/>
+      <c r="L78" t="s">
+        <v>1</v>
+      </c>
+      <c r="M78" t="s">
+        <v>2</v>
+      </c>
+      <c r="N78" t="s">
+        <v>3</v>
+      </c>
+      <c r="O78" t="s">
+        <v>220</v>
+      </c>
+      <c r="P78" t="s">
+        <v>5</v>
+      </c>
+      <c r="T78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L79">
+        <v>2</v>
+      </c>
+      <c r="M79">
+        <v>10.95</v>
+      </c>
+      <c r="N79">
+        <v>5.4729999999999999</v>
+      </c>
+      <c r="O79">
+        <v>2.2069999999999999</v>
+      </c>
+      <c r="P79">
+        <v>0.13</v>
+      </c>
+      <c r="T79" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="K80" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>0.64</v>
+      </c>
+      <c r="N80">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="O80">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="P80">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="T80" s="2"/>
+      <c r="U80" t="s">
+        <v>228</v>
+      </c>
+      <c r="V80" t="s">
+        <v>229</v>
+      </c>
+      <c r="W80" t="s">
+        <v>230</v>
+      </c>
+      <c r="X80" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K81" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81">
+        <v>26</v>
+      </c>
+      <c r="M81">
+        <v>64.48</v>
+      </c>
+      <c r="N81">
+        <v>2.48</v>
+      </c>
+      <c r="T81" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="U81" s="5">
+        <v>-1.3801416</v>
+      </c>
+      <c r="V81" s="5">
+        <v>-5.2026279999999998</v>
+      </c>
+      <c r="W81" s="5">
+        <v>2.442345</v>
+      </c>
+      <c r="X81" s="5">
+        <v>0.64849460000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T82" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="U82" s="5">
+        <v>-1.5011821000000001</v>
+      </c>
+      <c r="V82" s="5">
+        <v>-4.0035869999999996</v>
+      </c>
+      <c r="W82" s="5">
+        <v>1.0012228000000001</v>
+      </c>
+      <c r="X82" s="5">
+        <v>0.27807270000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T83" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="U83" s="5">
+        <v>-6.2028762999999998</v>
+      </c>
+      <c r="V83" s="5">
+        <v>-10.025363</v>
+      </c>
+      <c r="W83" s="5">
+        <v>-2.3803896999999998</v>
+      </c>
+      <c r="X83" s="5">
+        <v>4.4104000000000001E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T84" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="U84" s="5">
+        <v>-0.1210405</v>
+      </c>
+      <c r="V84" s="5">
+        <v>-4.2074509999999998</v>
+      </c>
+      <c r="W84" s="5">
+        <v>3.9653695999999998</v>
+      </c>
+      <c r="X84" s="5">
+        <v>0.99962850000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T85" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="U85" s="5">
+        <v>-4.8227346999999998</v>
+      </c>
+      <c r="V85" s="5">
+        <v>-9.8275439999999996</v>
+      </c>
+      <c r="W85" s="5">
+        <v>0.18207509999999999</v>
+      </c>
+      <c r="X85" s="5">
+        <v>5.84439E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T86" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="U86" s="5">
+        <v>-4.7016942000000004</v>
+      </c>
+      <c r="V86" s="5">
+        <v>-8.7881040000000006</v>
+      </c>
+      <c r="W86" s="5">
+        <v>-0.61528419999999995</v>
+      </c>
+      <c r="X86" s="5">
+        <v>2.6566800000000002E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
+      <c r="B94" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" t="s">
+        <v>217</v>
+      </c>
+      <c r="D94" t="s">
+        <v>218</v>
+      </c>
+      <c r="E94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" t="s">
+        <v>31</v>
+      </c>
+      <c r="G94" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95">
+        <v>3.2208000000000001</v>
+      </c>
+      <c r="D95">
+        <v>1.6104000000000001</v>
+      </c>
+      <c r="E95">
+        <v>10.131500000000001</v>
+      </c>
+      <c r="F95">
+        <v>0.13156000000000001</v>
+      </c>
+      <c r="G95">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0.81689999999999996</v>
+      </c>
+      <c r="D96">
+        <v>0.81689999999999996</v>
+      </c>
+      <c r="E96">
+        <v>5.1393000000000004</v>
+      </c>
+      <c r="F96">
+        <v>3.3369999999999997E-2</v>
+      </c>
+      <c r="G96">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97">
+        <v>2.8</v>
+      </c>
+      <c r="D97">
+        <v>1.40002</v>
+      </c>
+      <c r="E97">
+        <v>8.8079000000000001</v>
+      </c>
+      <c r="F97">
+        <v>0.11438</v>
+      </c>
+      <c r="G97">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98">
+        <v>111</v>
+      </c>
+      <c r="C98">
+        <v>17.6435</v>
+      </c>
+      <c r="D98">
+        <v>0.15895000000000001</v>
+      </c>
+      <c r="F98">
+        <v>0.72069000000000005</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99">
+        <v>116</v>
+      </c>
+      <c r="C99">
+        <v>24.481200000000001</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="2"/>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102">
+        <v>74.48</v>
+      </c>
+      <c r="D102">
+        <v>37.24</v>
+      </c>
+      <c r="E102">
+        <v>20.704000000000001</v>
+      </c>
+      <c r="F102" s="4">
+        <v>2.2799999999999999E-8</v>
+      </c>
+      <c r="G102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>182.1</v>
+      </c>
+      <c r="D103">
+        <v>91.05</v>
+      </c>
+      <c r="E103">
+        <v>50.622</v>
+      </c>
+      <c r="F103" s="4">
+        <v>2.3800000000000002E-16</v>
+      </c>
+      <c r="G103" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D104">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E104">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F104">
+        <v>0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105">
+        <v>111</v>
+      </c>
+      <c r="C105">
+        <v>199.64</v>
+      </c>
+      <c r="D105">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="2"/>
+      <c r="B114" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>3</v>
+      </c>
+      <c r="E114" t="s">
+        <v>220</v>
+      </c>
+      <c r="F114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>189.09</v>
+      </c>
+      <c r="D115">
+        <v>94.54</v>
+      </c>
+      <c r="E115">
+        <v>43.39</v>
+      </c>
+      <c r="F115" s="4">
+        <v>3.4000000000000002E-13</v>
+      </c>
+      <c r="G115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="C116">
+        <v>112.56</v>
+      </c>
+      <c r="D116">
+        <v>56.28</v>
+      </c>
+      <c r="E116">
+        <v>25.83</v>
+      </c>
+      <c r="F116" s="4">
+        <v>3.1E-9</v>
+      </c>
+      <c r="G116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>0.48</v>
+      </c>
+      <c r="D117">
+        <v>0.48</v>
+      </c>
+      <c r="E117">
+        <v>0.22</v>
+      </c>
+      <c r="F117">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118">
+        <v>74</v>
+      </c>
+      <c r="C118">
+        <v>161.24</v>
+      </c>
+      <c r="D118">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="2"/>
+      <c r="B120" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>28</v>
+      </c>
+      <c r="D120" t="s">
+        <v>29</v>
+      </c>
+      <c r="E120" t="s">
+        <v>30</v>
+      </c>
+      <c r="F120" t="s">
+        <v>31</v>
+      </c>
+      <c r="G120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+      <c r="C121" s="5">
+        <v>5.9687000000000001</v>
+      </c>
+      <c r="D121" s="5">
+        <v>2.9843600000000001</v>
+      </c>
+      <c r="E121" s="5">
+        <v>16.878699999999998</v>
+      </c>
+      <c r="F121" s="5">
+        <v>0.26889999999999997</v>
+      </c>
+      <c r="G121">
+        <v>1E-3</v>
+      </c>
+      <c r="H121" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122" s="5">
+        <v>0.3871</v>
+      </c>
+      <c r="D122" s="5">
+        <v>0.3871</v>
+      </c>
+      <c r="E122" s="5">
+        <v>2.1892999999999998</v>
+      </c>
+      <c r="F122" s="5">
+        <v>1.7440000000000001E-2</v>
+      </c>
+      <c r="G122">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H122" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="C123" s="5">
+        <v>2.7565</v>
+      </c>
+      <c r="D123" s="5">
+        <v>1.3782399999999999</v>
+      </c>
+      <c r="E123" s="5">
+        <v>7.7949000000000002</v>
+      </c>
+      <c r="F123" s="5">
+        <v>0.12418999999999999</v>
+      </c>
+      <c r="G123">
+        <v>1E-3</v>
+      </c>
+      <c r="H123" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>74</v>
+      </c>
+      <c r="C124" s="5">
+        <v>13.084099999999999</v>
+      </c>
+      <c r="D124" s="5">
+        <v>0.17680999999999999</v>
+      </c>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5">
+        <v>0.58947000000000005</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B125">
+        <v>79</v>
+      </c>
+      <c r="C125" s="5">
+        <v>22.196400000000001</v>
+      </c>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H158"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K148" sqref="K148"/>
+    <sheetView topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="A227" sqref="A227:G236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2934,6 +4467,902 @@
         <v>62</v>
       </c>
     </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A179" s="2"/>
+      <c r="B179" t="s">
+        <v>92</v>
+      </c>
+      <c r="C179" t="s">
+        <v>93</v>
+      </c>
+      <c r="D179" t="s">
+        <v>94</v>
+      </c>
+      <c r="E179" t="s">
+        <v>95</v>
+      </c>
+      <c r="F179" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B180" s="5">
+        <v>6.3453999999999997</v>
+      </c>
+      <c r="C180" s="5">
+        <v>0.78759999999999997</v>
+      </c>
+      <c r="D180" s="5">
+        <v>7.4141000000000004</v>
+      </c>
+      <c r="E180" s="5">
+        <v>8.0570000000000004</v>
+      </c>
+      <c r="F180" s="5">
+        <v>6.3600000000000001E-5</v>
+      </c>
+      <c r="G180" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B181" s="5">
+        <v>-1.2811999999999999</v>
+      </c>
+      <c r="C181" s="5">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="D181" s="5">
+        <v>6.4619</v>
+      </c>
+      <c r="E181" s="5">
+        <v>-1.444</v>
+      </c>
+      <c r="F181" s="5">
+        <v>0.19550000000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B182" s="5">
+        <v>-0.1016</v>
+      </c>
+      <c r="C182" s="5">
+        <v>1.0053000000000001</v>
+      </c>
+      <c r="D182" s="5">
+        <v>7.2561</v>
+      </c>
+      <c r="E182" s="5">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="F182" s="5">
+        <v>0.92230000000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B183" s="5">
+        <v>-0.28249999999999997</v>
+      </c>
+      <c r="C183" s="5">
+        <v>0.89170000000000005</v>
+      </c>
+      <c r="D183" s="5">
+        <v>6.5843999999999996</v>
+      </c>
+      <c r="E183" s="5">
+        <v>-0.317</v>
+      </c>
+      <c r="F183" s="5">
+        <v>0.76119999999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B184" s="5">
+        <v>-1.1995</v>
+      </c>
+      <c r="C184" s="5">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="D184" s="5">
+        <v>6.6506999999999996</v>
+      </c>
+      <c r="E184" s="5">
+        <v>-1.2210000000000001</v>
+      </c>
+      <c r="F184" s="5">
+        <v>0.26369999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A185" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B185" s="5">
+        <v>2.5594999999999999</v>
+      </c>
+      <c r="C185" s="5">
+        <v>1.0087999999999999</v>
+      </c>
+      <c r="D185" s="5">
+        <v>6.6234000000000002</v>
+      </c>
+      <c r="E185" s="5">
+        <v>2.5369999999999999</v>
+      </c>
+      <c r="F185" s="5">
+        <v>4.07E-2</v>
+      </c>
+      <c r="G185" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B186" s="5">
+        <v>0.73740000000000006</v>
+      </c>
+      <c r="C186" s="5">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="D186" s="5">
+        <v>6.4560000000000004</v>
+      </c>
+      <c r="E186" s="5">
+        <v>0.876</v>
+      </c>
+      <c r="F186" s="5">
+        <v>0.41220000000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B187" s="5">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="C187" s="5">
+        <v>0.69510000000000005</v>
+      </c>
+      <c r="D187" s="5">
+        <v>6.7385000000000002</v>
+      </c>
+      <c r="E187" s="5">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F187" s="5">
+        <v>0.65010000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B188" s="5">
+        <v>0.45140000000000002</v>
+      </c>
+      <c r="C188" s="5">
+        <v>0.24540000000000001</v>
+      </c>
+      <c r="D188" s="5">
+        <v>124.8702</v>
+      </c>
+      <c r="E188" s="5">
+        <v>1.839</v>
+      </c>
+      <c r="F188" s="5">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="G188" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A192" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A209" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A211" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A213" s="2"/>
+      <c r="B213" t="s">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s">
+        <v>28</v>
+      </c>
+      <c r="D213" t="s">
+        <v>29</v>
+      </c>
+      <c r="E213" t="s">
+        <v>30</v>
+      </c>
+      <c r="F213" t="s">
+        <v>31</v>
+      </c>
+      <c r="G213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A214" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B214">
+        <v>4</v>
+      </c>
+      <c r="C214">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="D214">
+        <v>1.17174</v>
+      </c>
+      <c r="E214">
+        <v>7.8249000000000004</v>
+      </c>
+      <c r="F214">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="G214">
+        <v>1E-3</v>
+      </c>
+      <c r="H214" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A215" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B215">
+        <v>3</v>
+      </c>
+      <c r="C215">
+        <v>4.3552</v>
+      </c>
+      <c r="D215">
+        <v>1.45173</v>
+      </c>
+      <c r="E215">
+        <v>9.6945999999999994</v>
+      </c>
+      <c r="F215">
+        <v>0.14551</v>
+      </c>
+      <c r="G215">
+        <v>1E-3</v>
+      </c>
+      <c r="H215" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A216" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>1.5705</v>
+      </c>
+      <c r="D216">
+        <v>1.5705100000000001</v>
+      </c>
+      <c r="E216">
+        <v>10.4878</v>
+      </c>
+      <c r="F216">
+        <v>5.2470000000000003E-2</v>
+      </c>
+      <c r="G216">
+        <v>1E-3</v>
+      </c>
+      <c r="H216" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A217" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B217">
+        <v>129</v>
+      </c>
+      <c r="C217">
+        <v>19.3172</v>
+      </c>
+      <c r="D217">
+        <v>0.14974999999999999</v>
+      </c>
+      <c r="F217">
+        <v>0.64541999999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A218" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B218">
+        <v>137</v>
+      </c>
+      <c r="C218">
+        <v>29.9299</v>
+      </c>
+      <c r="F218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A219" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A220" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A227" s="2"/>
+      <c r="B227" t="s">
+        <v>92</v>
+      </c>
+      <c r="C227" t="s">
+        <v>93</v>
+      </c>
+      <c r="D227" t="s">
+        <v>94</v>
+      </c>
+      <c r="E227" t="s">
+        <v>95</v>
+      </c>
+      <c r="F227" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A228" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B228" s="5">
+        <v>4.79108</v>
+      </c>
+      <c r="C228" s="5">
+        <v>1.02766</v>
+      </c>
+      <c r="D228" s="5">
+        <v>23.386579999999999</v>
+      </c>
+      <c r="E228" s="5">
+        <v>4.6619999999999999</v>
+      </c>
+      <c r="F228" s="5">
+        <v>1.0399999999999999E-4</v>
+      </c>
+      <c r="G228" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A229" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B229" s="5">
+        <v>-4.6086799999999997</v>
+      </c>
+      <c r="C229" s="5">
+        <v>0.92547000000000001</v>
+      </c>
+      <c r="D229" s="5">
+        <v>7.9817999999999998</v>
+      </c>
+      <c r="E229" s="5">
+        <v>-4.9800000000000004</v>
+      </c>
+      <c r="F229" s="5">
+        <v>1.0870000000000001E-3</v>
+      </c>
+      <c r="G229" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A230" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B230" s="5">
+        <v>-1.6423300000000001</v>
+      </c>
+      <c r="C230" s="5">
+        <v>0.90488999999999997</v>
+      </c>
+      <c r="D230" s="5">
+        <v>7.4087800000000001</v>
+      </c>
+      <c r="E230" s="5">
+        <v>-1.8149999999999999</v>
+      </c>
+      <c r="F230" s="5">
+        <v>0.110053</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A231" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B231" s="5">
+        <v>-0.89063000000000003</v>
+      </c>
+      <c r="C231" s="5">
+        <v>0.67325999999999997</v>
+      </c>
+      <c r="D231" s="5">
+        <v>6.5024499999999996</v>
+      </c>
+      <c r="E231" s="5">
+        <v>-1.323</v>
+      </c>
+      <c r="F231" s="5">
+        <v>0.23049900000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A232" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B232" s="5">
+        <v>-0.22450999999999999</v>
+      </c>
+      <c r="C232" s="5">
+        <v>1.07117</v>
+      </c>
+      <c r="D232" s="5">
+        <v>14.446289999999999</v>
+      </c>
+      <c r="E232" s="5">
+        <v>-0.21</v>
+      </c>
+      <c r="F232" s="5">
+        <v>0.83691000000000004</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A233" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B233" s="5">
+        <v>-1.4991699999999999</v>
+      </c>
+      <c r="C233" s="5">
+        <v>1.03854</v>
+      </c>
+      <c r="D233" s="5">
+        <v>12.27482</v>
+      </c>
+      <c r="E233" s="5">
+        <v>-1.444</v>
+      </c>
+      <c r="F233" s="5">
+        <v>0.173904</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B234" s="5">
+        <v>0.46378000000000003</v>
+      </c>
+      <c r="C234" s="5">
+        <v>1.0281199999999999</v>
+      </c>
+      <c r="D234" s="5">
+        <v>11.876060000000001</v>
+      </c>
+      <c r="E234" s="5">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="F234" s="5">
+        <v>0.66004600000000002</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A235" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B235" s="5">
+        <v>-1.8169999999999999E-2</v>
+      </c>
+      <c r="C235" s="5">
+        <v>0.96326999999999996</v>
+      </c>
+      <c r="D235" s="5">
+        <v>9.2179900000000004</v>
+      </c>
+      <c r="E235" s="5">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="F235" s="5">
+        <v>0.98534999999999995</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A236" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B236" s="5">
+        <v>1.2764800000000001</v>
+      </c>
+      <c r="C236" s="5">
+        <v>0.58203000000000005</v>
+      </c>
+      <c r="D236" s="5">
+        <v>75.740099999999998</v>
+      </c>
+      <c r="E236" s="5">
+        <v>2.1930000000000001</v>
+      </c>
+      <c r="F236" s="5">
+        <v>3.1365999999999998E-2</v>
+      </c>
+      <c r="G236" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A237" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A244" s="2"/>
+      <c r="B244" t="s">
+        <v>92</v>
+      </c>
+      <c r="C244" t="s">
+        <v>93</v>
+      </c>
+      <c r="D244" t="s">
+        <v>94</v>
+      </c>
+      <c r="E244" t="s">
+        <v>95</v>
+      </c>
+      <c r="F244" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A245" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B245">
+        <v>1.1574</v>
+      </c>
+      <c r="C245">
+        <v>0.223</v>
+      </c>
+      <c r="D245">
+        <v>15.787800000000001</v>
+      </c>
+      <c r="E245">
+        <v>5.19</v>
+      </c>
+      <c r="F245" s="4">
+        <v>9.3300000000000005E-5</v>
+      </c>
+      <c r="G245" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A246" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B246">
+        <v>1.0441</v>
+      </c>
+      <c r="C246">
+        <v>0.37409999999999999</v>
+      </c>
+      <c r="D246">
+        <v>21.251999999999999</v>
+      </c>
+      <c r="E246">
+        <v>2.7909999999999999</v>
+      </c>
+      <c r="F246">
+        <v>1.0869999999999999E-2</v>
+      </c>
+      <c r="G246" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A247" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B247">
+        <v>1.0028999999999999</v>
+      </c>
+      <c r="C247">
+        <v>0.33069999999999999</v>
+      </c>
+      <c r="D247">
+        <v>10.8019</v>
+      </c>
+      <c r="E247">
+        <v>3.032</v>
+      </c>
+      <c r="F247">
+        <v>1.162E-2</v>
+      </c>
+      <c r="G247" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A248" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B248">
+        <v>0.44619999999999999</v>
+      </c>
+      <c r="C248">
+        <v>0.29349999999999998</v>
+      </c>
+      <c r="D248">
+        <v>11.684699999999999</v>
+      </c>
+      <c r="E248">
+        <v>1.52</v>
+      </c>
+      <c r="F248">
+        <v>0.15498000000000001</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A249" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B249">
+        <v>-0.5131</v>
+      </c>
+      <c r="C249">
+        <v>0.1804</v>
+      </c>
+      <c r="D249">
+        <v>429.19810000000001</v>
+      </c>
+      <c r="E249">
+        <v>-2.8439999999999999</v>
+      </c>
+      <c r="F249">
+        <v>4.6699999999999997E-3</v>
+      </c>
+      <c r="G249" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A250" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B250">
+        <v>2.7004000000000001</v>
+      </c>
+      <c r="C250">
+        <v>0.1613</v>
+      </c>
+      <c r="D250">
+        <v>435.1671</v>
+      </c>
+      <c r="E250">
+        <v>16.741</v>
+      </c>
+      <c r="F250" t="s">
+        <v>184</v>
+      </c>
+      <c r="G250" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2942,175 +5371,390 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1674AE-ACC1-453C-AA37-C3459A9647D0}">
-  <dimension ref="A2:A38"/>
+  <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.5625</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.52810000000000001</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2.9590000000000001</v>
+      </c>
+      <c r="F13" s="5">
+        <v>4.0499999999999998E-3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-0.99919999999999998</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.58860000000000001</v>
+      </c>
+      <c r="E14" s="5">
+        <v>-1.698</v>
+      </c>
+      <c r="F14" s="5">
+        <v>9.3420000000000003E-2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="5">
+        <v>-1.157</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.67349999999999999</v>
+      </c>
+      <c r="E15" s="5">
+        <v>-1.718</v>
+      </c>
+      <c r="F15" s="5">
+        <v>8.9620000000000005E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.7484</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.63009999999999999</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2.7749999999999999</v>
+      </c>
+      <c r="F16" s="5">
+        <v>6.8500000000000002E-3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4.25</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.4703</v>
+      </c>
+      <c r="E17" s="5">
+        <v>9.0370000000000008</v>
+      </c>
+      <c r="F17" s="5">
+        <v>6.7099999999999999E-14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.47089999999999999</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.31524999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>5.6910999999999996</v>
+      </c>
+      <c r="D34">
+        <v>1.897</v>
+      </c>
+      <c r="E34">
+        <v>11.119400000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.24274999999999999</v>
+      </c>
+      <c r="G34">
+        <v>1E-3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="D35">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="E35">
+        <v>4.2977999999999996</v>
+      </c>
+      <c r="F35">
+        <v>3.1280000000000002E-2</v>
+      </c>
+      <c r="G35">
+        <v>2E-3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>3.2006999999999999</v>
+      </c>
+      <c r="D36">
+        <v>3.2006999999999999</v>
+      </c>
+      <c r="E36">
+        <v>18.7607</v>
+      </c>
+      <c r="F36">
+        <v>0.13652</v>
+      </c>
+      <c r="G36">
+        <v>1E-3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>81</v>
+      </c>
+      <c r="C37">
+        <v>13.819100000000001</v>
+      </c>
+      <c r="D37">
+        <v>0.1706</v>
+      </c>
+      <c r="F37">
+        <v>0.58945000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <v>86</v>
+      </c>
+      <c r="C38">
+        <v>23.444199999999999</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>163</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is a shitty commit with too much in it. I updated the report, split out the univariate stats by gear type, fixed the spelling on Sac-San Joaquin, and did some other stuff.
</commit_message>
<xml_diff>
--- a/PHaseIV analyses.xlsx
+++ b/PHaseIV analyses.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\FRPreport2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460456F5-E912-4D1E-B139-913B0B1D77FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28612732-2A14-4AFD-A8D5-76FCCD815E75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise" sheetId="1" r:id="rId1"/>
     <sheet name="decker time series" sheetId="4" r:id="rId2"/>
     <sheet name="IEP comparison" sheetId="5" r:id="rId3"/>
-    <sheet name="everything" sheetId="2" r:id="rId4"/>
-    <sheet name="spring v fall" sheetId="3" r:id="rId5"/>
+    <sheet name="phytoplankton" sheetId="6" r:id="rId4"/>
+    <sheet name="everything" sheetId="2" r:id="rId5"/>
+    <sheet name="spring v fall" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="296">
   <si>
     <t>---</t>
   </si>
@@ -797,6 +798,132 @@
   </si>
   <si>
     <t xml:space="preserve">-1.8075 -0.7965 -0.3960  0.5585  3.5815 </t>
+  </si>
+  <si>
+    <t>Associations between species and habitat types at Liberty Island</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>psidak</t>
+  </si>
+  <si>
+    <t>Achnanthidium sp.</t>
+  </si>
+  <si>
+    <t>Amphora sp.</t>
+  </si>
+  <si>
+    <t>Aulacoseira sp.</t>
+  </si>
+  <si>
+    <t>Biddulphia sp.</t>
+  </si>
+  <si>
+    <t>Cocconeis sp.</t>
+  </si>
+  <si>
+    <t>Cryptomonas sp.</t>
+  </si>
+  <si>
+    <t>Cyclotella sp.</t>
+  </si>
+  <si>
+    <t>Cymbella sp.</t>
+  </si>
+  <si>
+    <t>Diploneis sp.</t>
+  </si>
+  <si>
+    <t>Encyonema sp.</t>
+  </si>
+  <si>
+    <t>Epithemia sp.</t>
+  </si>
+  <si>
+    <t>Fragilaria sp.</t>
+  </si>
+  <si>
+    <t>Gomphonema sp.</t>
+  </si>
+  <si>
+    <t>Leptolyngbya sp.</t>
+  </si>
+  <si>
+    <t>Melosira sp.</t>
+  </si>
+  <si>
+    <t>Microcystis sp.</t>
+  </si>
+  <si>
+    <t>Monoraphidium arcuat</t>
+  </si>
+  <si>
+    <t>um                  0.300</t>
+  </si>
+  <si>
+    <t>Navicula sp.</t>
+  </si>
+  <si>
+    <t>Nitzschia sp.</t>
+  </si>
+  <si>
+    <t>Ochromonas sp.</t>
+  </si>
+  <si>
+    <t>Oscillatoria sp.</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Pandorina sp.</t>
+  </si>
+  <si>
+    <t>Rhoicosphenia sp.</t>
+  </si>
+  <si>
+    <t>Stephanodiscus sp.</t>
+  </si>
+  <si>
+    <t>Surirella sp.</t>
+  </si>
+  <si>
+    <t>Synedra sp.</t>
+  </si>
+  <si>
+    <t>Teleaulax sp.</t>
+  </si>
+  <si>
+    <t>Tetraspora sp.</t>
+  </si>
+  <si>
+    <t>Tychonema sp.</t>
+  </si>
+  <si>
+    <t>Pelagic</t>
+  </si>
+  <si>
+    <t>Benthic</t>
+  </si>
+  <si>
+    <t>SAV/FAV</t>
+  </si>
+  <si>
+    <t>Tules</t>
+  </si>
+  <si>
+    <t>Mysids only blitz</t>
+  </si>
+  <si>
+    <t>Sweepnets only blitz</t>
+  </si>
+  <si>
+    <t>TargetFAV</t>
+  </si>
+  <si>
+    <t>TargetSAV</t>
   </si>
 </sst>
 </file>
@@ -3246,7 +3373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94534BE3-97B1-4CFD-BD89-429247C6FEDC}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -3545,11 +3672,753 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF13F10-815D-44CC-9C28-F79DEA57B65B}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="A1:G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>0.995</v>
+      </c>
+      <c r="D3">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3">
+        <v>1.98505E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G4">
+        <v>1.98505E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5">
+        <v>1.98505E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D6">
+        <v>0.86</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>288</v>
+      </c>
+      <c r="G6">
+        <v>1.98505E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>0.98</v>
+      </c>
+      <c r="D7">
+        <v>0.79</v>
+      </c>
+      <c r="E7">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G7">
+        <v>1.98505E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.99</v>
+      </c>
+      <c r="E8">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G8">
+        <v>5.8663449999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.995</v>
+      </c>
+      <c r="D9">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G9">
+        <v>0.13281999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B10">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="D10">
+        <v>0.73</v>
+      </c>
+      <c r="E10">
+        <v>0.04</v>
+      </c>
+      <c r="F10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G10">
+        <v>0.15065344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>291</v>
+      </c>
+      <c r="G11">
+        <v>0.16821040000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12">
+        <v>0.62</v>
+      </c>
+      <c r="C12">
+        <v>0.05</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G12">
+        <v>0.18549375000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.83</v>
+      </c>
+      <c r="E13">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F13" t="s">
+        <v>289</v>
+      </c>
+      <c r="G13">
+        <v>0.20250635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.16</v>
+      </c>
+      <c r="E14">
+        <v>0.7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>288</v>
+      </c>
+      <c r="G14">
+        <v>0.25194799000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0.37</v>
+      </c>
+      <c r="D15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>290</v>
+      </c>
+      <c r="G15">
+        <v>0.26790586</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C16">
+        <v>0.08</v>
+      </c>
+      <c r="D16">
+        <v>0.215</v>
+      </c>
+      <c r="E16">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="F16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G16">
+        <v>0.28360703999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="C17">
+        <v>0.09</v>
+      </c>
+      <c r="D17">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F17" t="s">
+        <v>289</v>
+      </c>
+      <c r="G17">
+        <v>0.31425038999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18">
+        <v>0.625</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.105</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>290</v>
+      </c>
+      <c r="G18">
+        <v>0.35835895000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19">
+        <v>0.64</v>
+      </c>
+      <c r="C19">
+        <v>0.105</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>289</v>
+      </c>
+      <c r="G19">
+        <v>0.35835895000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C20">
+        <v>0.99</v>
+      </c>
+      <c r="D20">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="E20">
+        <v>0.115</v>
+      </c>
+      <c r="F20" t="s">
+        <v>291</v>
+      </c>
+      <c r="G20">
+        <v>0.38655859999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="C21">
+        <v>0.315</v>
+      </c>
+      <c r="D21">
+        <v>0.13</v>
+      </c>
+      <c r="E21">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F21" t="s">
+        <v>290</v>
+      </c>
+      <c r="G21">
+        <v>0.42710239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.18</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>290</v>
+      </c>
+      <c r="G22">
+        <v>0.54787823999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.185</v>
+      </c>
+      <c r="F23" t="s">
+        <v>291</v>
+      </c>
+      <c r="G23">
+        <v>0.55880514999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G24">
+        <v>0.60054439999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D25">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>289</v>
+      </c>
+      <c r="G25">
+        <v>0.60054439999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C26">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>288</v>
+      </c>
+      <c r="G26">
+        <v>0.65751170000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F27" t="s">
+        <v>291</v>
+      </c>
+      <c r="G27">
+        <v>0.65751170000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B28">
+        <v>0.34</v>
+      </c>
+      <c r="C28">
+        <v>0.43</v>
+      </c>
+      <c r="D28">
+        <v>0.24</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>290</v>
+      </c>
+      <c r="G28">
+        <v>0.66637824000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B29">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="C29">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D29">
+        <v>0.255</v>
+      </c>
+      <c r="E29">
+        <v>0.34</v>
+      </c>
+      <c r="F29" t="s">
+        <v>290</v>
+      </c>
+      <c r="G29">
+        <v>0.69194725000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B30">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>288</v>
+      </c>
+      <c r="G30">
+        <v>0.80443704999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D31">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E31">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>289</v>
+      </c>
+      <c r="G31">
+        <v>0.81593755000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B32">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>288</v>
+      </c>
+      <c r="G32">
+        <v>0.85694585000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G32">
+    <sortCondition ref="G3:G32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H250"/>
+  <dimension ref="A1:H268"/>
   <sheetViews>
-    <sheetView topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="A227" sqref="A227:G236"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="A262" sqref="A262:G268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6060,13 +6929,283 @@
         <v>7</v>
       </c>
     </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A255" s="2"/>
+      <c r="B255" t="s">
+        <v>92</v>
+      </c>
+      <c r="C255" t="s">
+        <v>93</v>
+      </c>
+      <c r="D255" t="s">
+        <v>94</v>
+      </c>
+      <c r="E255" t="s">
+        <v>95</v>
+      </c>
+      <c r="F255" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A256" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B256">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="C256">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D256">
+        <v>12.370699999999999</v>
+      </c>
+      <c r="E256">
+        <v>3.5609999999999999</v>
+      </c>
+      <c r="F256">
+        <v>3.7399999999999998E-3</v>
+      </c>
+      <c r="G256" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A257" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B257">
+        <v>1.0789</v>
+      </c>
+      <c r="C257">
+        <v>0.30659999999999998</v>
+      </c>
+      <c r="D257">
+        <v>9.3652999999999995</v>
+      </c>
+      <c r="E257">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="F257">
+        <v>6.13E-3</v>
+      </c>
+      <c r="G257" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A258" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B258">
+        <v>0.42720000000000002</v>
+      </c>
+      <c r="C258">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="D258">
+        <v>9.6402000000000001</v>
+      </c>
+      <c r="E258">
+        <v>1.57</v>
+      </c>
+      <c r="F258">
+        <v>0.14854999999999999</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A259" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B259">
+        <v>0.5171</v>
+      </c>
+      <c r="C259">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D259">
+        <v>122.1982</v>
+      </c>
+      <c r="E259">
+        <v>2.532</v>
+      </c>
+      <c r="F259">
+        <v>1.26E-2</v>
+      </c>
+      <c r="G259" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A261" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A262" s="2"/>
+      <c r="B262" t="s">
+        <v>92</v>
+      </c>
+      <c r="C262" t="s">
+        <v>93</v>
+      </c>
+      <c r="D262" t="s">
+        <v>94</v>
+      </c>
+      <c r="E262" t="s">
+        <v>95</v>
+      </c>
+      <c r="F262" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A263" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B263">
+        <v>3.1227999999999998</v>
+      </c>
+      <c r="C263">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D263">
+        <v>11.8857</v>
+      </c>
+      <c r="E263">
+        <v>9.5510000000000002</v>
+      </c>
+      <c r="F263" s="4">
+        <v>6.3399999999999999E-7</v>
+      </c>
+      <c r="G263" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A264" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B264">
+        <v>1.4232</v>
+      </c>
+      <c r="C264">
+        <v>0.2571</v>
+      </c>
+      <c r="D264">
+        <v>192.226</v>
+      </c>
+      <c r="E264">
+        <v>5.5359999999999996</v>
+      </c>
+      <c r="F264" s="4">
+        <v>1.01E-7</v>
+      </c>
+      <c r="G264" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A265" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B265">
+        <v>2.1970999999999998</v>
+      </c>
+      <c r="C265">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="D265">
+        <v>191.9606</v>
+      </c>
+      <c r="E265">
+        <v>8.7289999999999992</v>
+      </c>
+      <c r="F265" s="4">
+        <v>1.24E-15</v>
+      </c>
+      <c r="G265" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A266" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B266">
+        <v>1.5483</v>
+      </c>
+      <c r="C266">
+        <v>0.495</v>
+      </c>
+      <c r="D266">
+        <v>11.385899999999999</v>
+      </c>
+      <c r="E266">
+        <v>3.1280000000000001</v>
+      </c>
+      <c r="F266">
+        <v>9.2499999999999995E-3</v>
+      </c>
+      <c r="G266" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B267">
+        <v>0.89039999999999997</v>
+      </c>
+      <c r="C267">
+        <v>0.47089999999999999</v>
+      </c>
+      <c r="D267">
+        <v>9.4315999999999995</v>
+      </c>
+      <c r="E267">
+        <v>1.891</v>
+      </c>
+      <c r="F267">
+        <v>8.9690000000000006E-2</v>
+      </c>
+      <c r="G267" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B268">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="C268">
+        <v>0.4279</v>
+      </c>
+      <c r="D268">
+        <v>10.5153</v>
+      </c>
+      <c r="E268">
+        <v>1.621</v>
+      </c>
+      <c r="F268">
+        <v>0.13469</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1674AE-ACC1-453C-AA37-C3459A9647D0}">
   <dimension ref="A2:H40"/>
   <sheetViews>

</xml_diff>